<commit_message>
update data sheets, initial figures notebook
</commit_message>
<xml_diff>
--- a/data/processed/CascadiaMargin_index_values.xlsx
+++ b/data/processed/CascadiaMargin_index_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/cascadia-margin-lipids/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/cascadia-margin-lipids/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99C2BD8-5D01-844F-9332-566CC3E5C976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847F152D-2DB8-F943-ACBF-D311C12279E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="7020" windowWidth="13980" windowHeight="13420" xr2:uid="{8DD774BC-1906-1E41-9886-58525280DC81}"/>
+    <workbookView xWindow="4700" yWindow="1180" windowWidth="32660" windowHeight="21380" xr2:uid="{8DD774BC-1906-1E41-9886-58525280DC81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Location</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>S113</t>
+  </si>
+  <si>
+    <t>delta_sst</t>
+  </si>
+  <si>
+    <t>50th_percentile</t>
   </si>
 </sst>
 </file>
@@ -255,11 +261,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -279,9 +291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -319,7 +331,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -425,7 +437,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,15 +587,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A67AC7-AD91-FA4A-BD47-9F4A66AF22B1}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -593,17 +605,23 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -613,17 +631,24 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0.66898897089939002</v>
+      <c r="D2" s="5">
+        <v>0.67720575362318292</v>
       </c>
       <c r="E2">
         <v>0.48252283468287599</v>
       </c>
-      <c r="F2">
-        <v>0.48699293309134217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="7">
+        <v>0.47675468958626593</v>
+      </c>
+      <c r="G2">
+        <v>24.517788605689201</v>
+      </c>
+      <c r="H2">
+        <f>G2-15.56</f>
+        <v>8.9577886056892009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -633,17 +658,24 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>0.57641256206554359</v>
+      <c r="D3" s="5">
+        <v>0.5868567624647687</v>
       </c>
       <c r="E3">
         <v>0.45166681430618888</v>
       </c>
-      <c r="F3">
-        <v>0.4813387751426334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="7">
+        <v>0.48594658278166525</v>
+      </c>
+      <c r="G3">
+        <v>18.918613182019001</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H38" si="0">G3-15.56</f>
+        <v>3.3586131820190008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -653,17 +685,24 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>0.62766803662230974</v>
+      <c r="D4" s="5">
+        <v>0.63185726321298019</v>
       </c>
       <c r="E4">
-        <v>0.43062397852445133</v>
-      </c>
-      <c r="F4">
-        <v>0.578407859979856</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.43081878714872546</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.56700657936281273</v>
+      </c>
+      <c r="G4">
+        <v>21.974243864001402</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>6.414243864001401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -673,17 +712,24 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0.62654188164718772</v>
+      <c r="D5" s="5">
+        <v>0.63219372691698583</v>
       </c>
       <c r="E5">
-        <v>0.42365114287481942</v>
-      </c>
-      <c r="F5">
-        <v>0.74758272863711506</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.42281505381099865</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.7376073587455062</v>
+      </c>
+      <c r="G5">
+        <v>21.9115919431406</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>6.3515919431405994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -693,17 +739,24 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
-        <v>0.6661689887295571</v>
+      <c r="D6" s="5">
+        <v>0.65692697188887328</v>
       </c>
       <c r="E6">
-        <v>0.45516333995045749</v>
-      </c>
-      <c r="F6">
-        <v>0.4911430704272931</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.45519670545808366</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.46305351519692262</v>
+      </c>
+      <c r="G6">
+        <v>24.310981209569299</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>8.7509812095692983</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -713,17 +766,24 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>0.76928947089430288</v>
+      <c r="D7" s="5">
+        <v>0.76449179000999357</v>
       </c>
       <c r="E7">
-        <v>0.43956232151397273</v>
-      </c>
-      <c r="F7">
-        <v>0.70340412034440736</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.43944510919145563</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.67147613962434949</v>
+      </c>
+      <c r="G7">
+        <v>30.604425181995499</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>15.044425181995498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -733,17 +793,24 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8">
-        <v>0.79154494174577172</v>
+      <c r="D8" s="5">
+        <v>0.77858697708256275</v>
       </c>
       <c r="E8">
-        <v>0.4408509830284395</v>
-      </c>
-      <c r="F8">
-        <v>0.73441258555276112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.43671128266235232</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.70139947618082699</v>
+      </c>
+      <c r="G8">
+        <v>32.176226092316298</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>16.616226092316296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -753,17 +820,24 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9">
-        <v>0.79328733652776107</v>
+      <c r="D9" s="5">
+        <v>0.77797321843015677</v>
       </c>
       <c r="E9">
-        <v>0.46921780736444568</v>
-      </c>
-      <c r="F9">
-        <v>0.79403741649868298</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.4684781483875734</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.76047110727067635</v>
+      </c>
+      <c r="G9">
+        <v>32.131591673939297</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>16.571591673939295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -773,17 +847,24 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>0.61002859807289811</v>
+      <c r="D10" s="5">
+        <v>0.61012813547165423</v>
       </c>
       <c r="E10">
         <v>0.35556454140414756</v>
       </c>
-      <c r="F10">
-        <v>0.2744449962421267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="7">
+        <v>0.28689556348515072</v>
+      </c>
+      <c r="G10">
+        <v>21.1457808641524</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5.5857808641523992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -793,17 +874,24 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>0.65615332229434464</v>
+      <c r="D11" s="5">
+        <v>0.62464708172255301</v>
       </c>
       <c r="E11">
-        <v>0.33186886653253617</v>
-      </c>
-      <c r="F11">
-        <v>0.33527828007065352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.7554682824761093E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.3232576483163408</v>
+      </c>
+      <c r="G11">
+        <v>23.797948646557298</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>8.2379486465572977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -813,17 +901,24 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>0.59512295340051236</v>
+      <c r="D12" s="5">
+        <v>0.59826042423482273</v>
       </c>
       <c r="E12">
-        <v>0.33896373963456627</v>
-      </c>
-      <c r="F12">
-        <v>0.29487897840627419</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.4366285293107131E-2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.29284137025907736</v>
+      </c>
+      <c r="G12">
+        <v>19.975727546707599</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>4.4157275467075987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -833,17 +928,24 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13">
-        <v>0.55738760084192962</v>
+      <c r="D13" s="5">
+        <v>0.55679482574771211</v>
       </c>
       <c r="E13">
         <v>0.32249837750848853</v>
       </c>
-      <c r="F13">
-        <v>0.33025856434469175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="7">
+        <v>0.32996151375652949</v>
+      </c>
+      <c r="G13">
+        <v>17.918391450992001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2.3583914509920003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -853,17 +955,24 @@
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14">
-        <v>0.66316492821117423</v>
+      <c r="D14" s="5">
+        <v>0.65104674118680617</v>
       </c>
       <c r="E14">
-        <v>0.27827163388924503</v>
-      </c>
-      <c r="F14">
-        <v>0.72596649680068437</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.5601082960786414E-2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.72151193175048589</v>
+      </c>
+      <c r="G14">
+        <v>24.233541536736102</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>8.6735415367361011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -873,17 +982,24 @@
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15">
-        <v>0.59731454241936377</v>
+      <c r="D15" s="5">
+        <v>0.58745651548337741</v>
       </c>
       <c r="E15">
-        <v>0.32577487919175663</v>
-      </c>
-      <c r="F15">
-        <v>0.35792194267189814</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.985109953863565E-2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.36046417895832011</v>
+      </c>
+      <c r="G15">
+        <v>20.315739032769599</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>4.7557390327695988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -893,17 +1009,24 @@
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16">
-        <v>0.56252946394761139</v>
+      <c r="D16" s="5">
+        <v>0.61471232584389945</v>
       </c>
       <c r="E16">
-        <v>0.29975936144079895</v>
-      </c>
-      <c r="F16">
-        <v>0.30671656652092832</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.9301981181731859E-2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.29779406554455229</v>
+      </c>
+      <c r="G16">
+        <v>18.211894451930998</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>2.6518944519309979</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -913,17 +1036,24 @@
       <c r="C17">
         <v>10</v>
       </c>
-      <c r="D17">
-        <v>0.56713648619121471</v>
+      <c r="D17" s="5">
+        <v>0.50150904559058185</v>
       </c>
       <c r="E17">
-        <v>0.39808557288084706</v>
-      </c>
-      <c r="F17">
-        <v>0.29955403723861362</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.6268064653699753E-2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.29925288745092726</v>
+      </c>
+      <c r="G17">
+        <v>18.3198261643969</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>2.7598261643969</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -933,17 +1063,24 @@
       <c r="C18">
         <v>30</v>
       </c>
-      <c r="D18">
-        <v>0.58323604059658407</v>
+      <c r="D18" s="5">
+        <v>0.5773854410165693</v>
       </c>
       <c r="E18">
-        <v>0.34866878845536292</v>
-      </c>
-      <c r="F18">
-        <v>0.30414753122423854</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9.0561564958728732E-2</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.3096004709373002</v>
+      </c>
+      <c r="G18">
+        <v>19.379193723721201</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>3.8191937237212006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -953,17 +1090,24 @@
       <c r="C19">
         <v>30</v>
       </c>
-      <c r="D19">
-        <v>0.57216399842282062</v>
+      <c r="D19" s="5">
+        <v>0.58382490891929728</v>
       </c>
       <c r="E19">
-        <v>0.37262738267206558</v>
-      </c>
-      <c r="F19">
-        <v>0.3171894342715243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.3991924743458115E-2</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.3119960168121429</v>
+      </c>
+      <c r="G19">
+        <v>18.7931499324378</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>3.233149932437799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -973,17 +1117,24 @@
       <c r="C20">
         <v>30</v>
       </c>
-      <c r="D20">
-        <v>0.54201797599344315</v>
+      <c r="D20" s="5">
+        <v>0.47155901673549244</v>
       </c>
       <c r="E20">
-        <v>0.36656593035824325</v>
-      </c>
-      <c r="F20">
-        <v>0.28509710599782406</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.5108561103626778E-2</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.27547075959207301</v>
+      </c>
+      <c r="G20">
+        <v>16.8056329437802</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1.2456329437801994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -993,17 +1144,24 @@
       <c r="C21">
         <v>30</v>
       </c>
-      <c r="D21">
-        <v>0.58328641573439743</v>
+      <c r="D21" s="5">
+        <v>0.57776550949610006</v>
       </c>
       <c r="E21">
-        <v>0.36136615387023657</v>
-      </c>
-      <c r="F21">
-        <v>0.28063117144600108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.3765614949241354E-2</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.28041980692485835</v>
+      </c>
+      <c r="G21">
+        <v>19.327188492201198</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>3.767188492201198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1013,17 +1171,24 @@
       <c r="C22">
         <v>60</v>
       </c>
-      <c r="D22">
-        <v>0.58422436939346267</v>
+      <c r="D22" s="5">
+        <v>0.54173696060728427</v>
       </c>
       <c r="E22">
-        <v>0.42105837169244081</v>
-      </c>
-      <c r="F22">
-        <v>0.22778935808551889</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.963599031999182E-2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.21844802213791911</v>
+      </c>
+      <c r="G22">
+        <v>19.2749344444432</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>3.7149344444432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1033,17 +1198,24 @@
       <c r="C23">
         <v>60</v>
       </c>
-      <c r="D23">
-        <v>0.62703340623808024</v>
+      <c r="D23" s="5">
+        <v>0.57122520382548236</v>
       </c>
       <c r="E23">
         <v>0.44013059778514702</v>
       </c>
-      <c r="F23">
-        <v>0.29650384239423044</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="7">
+        <v>0.2899238250932229</v>
+      </c>
+      <c r="G23">
+        <v>21.955062362703899</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>6.3950623627038983</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1053,17 +1225,24 @@
       <c r="C24">
         <v>60</v>
       </c>
-      <c r="D24">
-        <v>0.62976674467504301</v>
+      <c r="D24" s="5">
+        <v>0.61807051359432152</v>
       </c>
       <c r="E24">
-        <v>0.41873469352054826</v>
-      </c>
-      <c r="F24">
-        <v>0.25983883134024127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.2090646911864832E-2</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.26298849811163255</v>
+      </c>
+      <c r="G24">
+        <v>21.934208374188401</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>6.3742083741884006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1073,17 +1252,24 @@
       <c r="C25">
         <v>60</v>
       </c>
-      <c r="D25">
-        <v>0.59511332596690147</v>
+      <c r="D25" s="5">
+        <v>0.6066447599408209</v>
       </c>
       <c r="E25">
-        <v>0.38379666181687383</v>
-      </c>
-      <c r="F25">
-        <v>0.25641198966387713</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.8422642092251615E-2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.25233588885542452</v>
+      </c>
+      <c r="G25">
+        <v>19.9948360298919</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>4.4348360298918994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -1093,17 +1279,24 @@
       <c r="C26">
         <v>15</v>
       </c>
-      <c r="D26">
-        <v>0.47057167577841774</v>
+      <c r="D26" s="5">
+        <v>0.45720341465494868</v>
       </c>
       <c r="E26">
-        <v>0.41345251605058153</v>
-      </c>
-      <c r="F26">
-        <v>0.19665181321272995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.7516495966536527E-2</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.19868234179774921</v>
+      </c>
+      <c r="G26">
+        <v>12.371556637357299</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>-3.1884433626427011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1113,17 +1306,24 @@
       <c r="C27">
         <v>30</v>
       </c>
-      <c r="D27">
-        <v>0.43528275607241412</v>
+      <c r="D27" s="5">
+        <v>0.41756755012391528</v>
       </c>
       <c r="E27">
-        <v>0.46675097869306076</v>
-      </c>
-      <c r="F27">
-        <v>0.21574158329760967</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.3057298328687468E-2</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.22366057251142091</v>
+      </c>
+      <c r="G27">
+        <v>10.5080314660926</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>-5.0519685339074005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1133,17 +1333,24 @@
       <c r="C28">
         <v>30</v>
       </c>
-      <c r="D28">
-        <v>0.49196061152473991</v>
+      <c r="D28" s="5">
+        <v>0.48926204697178849</v>
       </c>
       <c r="E28">
-        <v>0.45611314717445228</v>
-      </c>
-      <c r="F28">
-        <v>0.20440116040090844</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.3613081103649109E-2</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.20315729505347366</v>
+      </c>
+      <c r="G28">
+        <v>13.791257926320201</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>-1.7687420736797996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1153,17 +1360,24 @@
       <c r="C29">
         <v>30</v>
       </c>
-      <c r="D29">
-        <v>0.45669554737920115</v>
+      <c r="D29" s="5">
+        <v>0.45458045581977785</v>
       </c>
       <c r="E29">
-        <v>0.45479366250735975</v>
-      </c>
-      <c r="F29">
-        <v>0.21266584154074664</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.9441976144376328E-2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.21389886908642072</v>
+      </c>
+      <c r="G29">
+        <v>11.642581291313499</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>-3.9174187086865011</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -1173,17 +1387,24 @@
       <c r="C30">
         <v>30</v>
       </c>
-      <c r="D30">
-        <v>0.48129599438443599</v>
+      <c r="D30" s="5">
+        <v>0.48317909607307613</v>
       </c>
       <c r="E30">
-        <v>0.43591296559682507</v>
-      </c>
-      <c r="F30">
-        <v>0.20419899489980287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.8248092889005999E-2</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.20425247150247222</v>
+      </c>
+      <c r="G30">
+        <v>13.352245686270701</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>-2.2077543137292999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1193,17 +1414,24 @@
       <c r="C31">
         <v>60</v>
       </c>
-      <c r="D31">
-        <v>0.46756108655554551</v>
+      <c r="D31" s="5">
+        <v>0.44453464866875081</v>
       </c>
       <c r="E31">
-        <v>0.43436217318556569</v>
-      </c>
-      <c r="F31">
-        <v>0.19337398885350482</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.3954684179315416E-2</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.19604336213331397</v>
+      </c>
+      <c r="G31">
+        <v>12.3689527710367</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>-3.191047228963301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1213,17 +1441,24 @@
       <c r="C32">
         <v>60</v>
       </c>
-      <c r="D32">
-        <v>0.4273876849995531</v>
+      <c r="D32" s="5">
+        <v>0.43940722611414484</v>
       </c>
       <c r="E32">
-        <v>0.47520101580157598</v>
-      </c>
-      <c r="F32">
-        <v>0.20192158486361669</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.8826180099903659E-2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.20173032790264581</v>
+      </c>
+      <c r="G32">
+        <v>9.8781657039055908</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>-5.6818342960944097</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1233,17 +1468,24 @@
       <c r="C33">
         <v>60</v>
       </c>
-      <c r="D33">
-        <v>0.4395735235911899</v>
+      <c r="D33" s="5">
+        <v>0.46028391362290083</v>
       </c>
       <c r="E33">
-        <v>0.44961156059860985</v>
-      </c>
-      <c r="F33">
-        <v>0.20137760096997548</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.3229116749378334E-2</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.19712664133441202</v>
+      </c>
+      <c r="G33">
+        <v>10.749016627219</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>-4.810983372781001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1253,17 +1495,24 @@
       <c r="C34">
         <v>60</v>
       </c>
-      <c r="D34">
-        <v>0.44067515392780549</v>
+      <c r="D34" s="5">
+        <v>0.44655273777774895</v>
       </c>
       <c r="E34">
-        <v>0.43578405472264492</v>
-      </c>
-      <c r="F34">
-        <v>0.21562367619404835</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.8030581015928691E-2</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.21598927108681895</v>
+      </c>
+      <c r="G34">
+        <v>10.754173761845299</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>-4.805826238154701</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1273,17 +1522,24 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0.47714729098208275</v>
+      <c r="D35" s="5">
+        <v>0.4681156752644125</v>
       </c>
       <c r="E35">
-        <v>0.50558871812756068</v>
-      </c>
-      <c r="F35">
-        <v>0.20191503028999105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.2744656598234698E-2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.20634415418287913</v>
+      </c>
+      <c r="G35">
+        <v>12.730642208976599</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>-2.8293577910234013</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1293,17 +1549,24 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>0.4463273611581734</v>
+      <c r="D36" s="5">
+        <v>0.44638196588260742</v>
       </c>
       <c r="E36">
-        <v>0.47106003350354969</v>
-      </c>
-      <c r="F36">
-        <v>0.22683857026136564</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.9942628624475413E-2</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.22749635560191175</v>
+      </c>
+      <c r="G36">
+        <v>10.9753925655431</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>-4.5846074344569008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1313,17 +1576,24 @@
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37">
-        <v>0.51517772250329463</v>
+      <c r="D37" s="5">
+        <v>0.51252808105275394</v>
       </c>
       <c r="E37">
-        <v>0.45640778578093943</v>
-      </c>
-      <c r="F37">
-        <v>0.22601127825340453</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.9732792777112579E-2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.22582640766859632</v>
+      </c>
+      <c r="G37">
+        <v>15.1548343950268</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>-0.40516560497320064</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1333,14 +1603,21 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38">
-        <v>0.51537300698459299</v>
+      <c r="D38" s="5">
+        <v>0.50995610213373854</v>
       </c>
       <c r="E38">
-        <v>0.44613840917517117</v>
-      </c>
-      <c r="F38">
-        <v>0.22341331427260133</v>
+        <v>8.183109748619094E-2</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.22425042449442903</v>
+      </c>
+      <c r="G38">
+        <v>15.3387246784964</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>-0.22127532150360096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>